<commit_message>
i318--reveal suite file update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
@@ -25,18 +25,18 @@
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
   <customWorkbookViews>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="441">
   <si>
     <t>CaseInfo</t>
   </si>
@@ -1348,7 +1348,49 @@
     <t>radiant=ng2_3</t>
   </si>
   <si>
-    <t>debug_10_reveal_inserter_v2.00</t>
+    <t>debug_10_reveal_inserter_v2.01</t>
+  </si>
+  <si>
+    <t>HDL_syntax/00_device_flow/01_Thunderplus</t>
+  </si>
+  <si>
+    <t>Device_coverage</t>
+  </si>
+  <si>
+    <t>device coverage: Thunderplus</t>
+  </si>
+  <si>
+    <t>HDL_syntax/00_device_flow/02_Jedi</t>
+  </si>
+  <si>
+    <t>device coverage: Jedi</t>
+  </si>
+  <si>
+    <t>HDL_syntax/00_device_flow/03_Jedi_D2</t>
+  </si>
+  <si>
+    <t>device coverage: Jedi_D2</t>
+  </si>
+  <si>
+    <t>HDL_syntax/00_device_flow/04_Jedi_D1</t>
+  </si>
+  <si>
+    <t>device coverage: Jedi_D1</t>
+  </si>
+  <si>
+    <t>cmd= --run-export-bitstream</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
   </si>
 </sst>
 </file>
@@ -5253,7 +5295,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{41778547-DEA6-4E5D-9DAF-FB4EF3474EA0}" diskRevisions="1" revisionId="498" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A4822E2F-5A05-4643-84A4-810DB5F4877E}" diskRevisions="1" revisionId="530" version="12">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5326,11 +5368,268 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{E6B56078-3384-4A26-82EC-5A857212A755}" dateTime="2021-02-01T13:42:29" maxSheetId="5" userName="Jason Wang" r:id="rId10" minRId="499" maxRId="523">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CA92E75E-BB28-4DE7-925B-1F96DD6335EB}" dateTime="2021-02-01T13:42:45" maxSheetId="5" userName="Jason Wang" r:id="rId11" minRId="525" maxRId="528">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A4822E2F-5A05-4643-84A4-810DB5F4877E}" dateTime="2021-02-01T13:42:49" maxSheetId="5" userName="Jason Wang" r:id="rId12">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="499" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.00</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.01</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="500" sId="2">
+    <nc r="D84" t="inlineStr">
+      <is>
+        <t>Device_coverage</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="501" sId="2">
+    <nc r="E84" t="inlineStr">
+      <is>
+        <t>HDL_syntax/00_device_flow/01_Thunderplus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="502" sId="2">
+    <nc r="H84" t="inlineStr">
+      <is>
+        <t>device coverage: Thunderplus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="503" sId="2">
+    <nc r="D85" t="inlineStr">
+      <is>
+        <t>Device_coverage</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="504" sId="2">
+    <nc r="E85" t="inlineStr">
+      <is>
+        <t>HDL_syntax/00_device_flow/02_Jedi</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="505" sId="2">
+    <nc r="H85" t="inlineStr">
+      <is>
+        <t>device coverage: Jedi</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="506" sId="2">
+    <nc r="D86" t="inlineStr">
+      <is>
+        <t>Device_coverage</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="507" sId="2">
+    <nc r="E86" t="inlineStr">
+      <is>
+        <t>HDL_syntax/00_device_flow/03_Jedi_D2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="508" sId="2">
+    <nc r="H86" t="inlineStr">
+      <is>
+        <t>device coverage: Jedi_D2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="509" sId="2">
+    <nc r="D87" t="inlineStr">
+      <is>
+        <t>Device_coverage</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="510" sId="2">
+    <nc r="E87" t="inlineStr">
+      <is>
+        <t>HDL_syntax/00_device_flow/04_Jedi_D1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="511" sId="2">
+    <nc r="H87" t="inlineStr">
+      <is>
+        <t>device coverage: Jedi_D1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="512" sId="2" numFmtId="30">
+    <nc r="F84">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="513" sId="2" numFmtId="30">
+    <nc r="F85">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="514" sId="2" numFmtId="30">
+    <nc r="F86">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="515" sId="2" numFmtId="30">
+    <nc r="F87">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="516" sId="2">
+    <nc r="O84" t="inlineStr">
+      <is>
+        <t>cmd= --run-export-bitstream</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="517" sId="2">
+    <nc r="O85" t="inlineStr">
+      <is>
+        <t>cmd= --run-export-bitstream</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="518" sId="2">
+    <nc r="O86" t="inlineStr">
+      <is>
+        <t>cmd= --run-export-bitstream</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="519" sId="2">
+    <nc r="O87" t="inlineStr">
+      <is>
+        <t>cmd= --run-export-bitstream</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="520" sId="2">
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="521" sId="2">
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>83</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="522" sId="2">
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>84</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="523" sId="2">
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="525" sId="2">
+    <nc r="S84" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="526" sId="2">
+    <nc r="S85" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="527" sId="2">
+    <nc r="S86" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="528" sId="2">
+    <nc r="S87" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9058,9 +9357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -9161,7 +9458,7 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -9174,14 +9471,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD83"/>
+  <dimension ref="A1:AD87"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10718,6 +11015,98 @@
         <v>264</v>
       </c>
     </row>
+    <row r="84" spans="1:19">
+      <c r="A84" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F84" s="2">
+        <v>2</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="O84" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="S84" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
+      <c r="A85" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F85" s="2">
+        <v>2</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="S85" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
+      <c r="A86" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="F86" s="2">
+        <v>2</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
+      <c r="A87" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="F87" s="2">
+        <v>2</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
@@ -10744,8 +11133,8 @@
       <autoFilter ref="A2:AD2"/>
     </customSheetView>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
       <autoFilter ref="A2:AD2"/>

</xml_diff>

<commit_message>
i334--Suite file reveal_inserter update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
@@ -27,16 +27,16 @@
   </definedNames>
   <calcPr calcId="122211" calcOnSave="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="444">
   <si>
     <t>CaseInfo</t>
   </si>
@@ -1345,12 +1345,6 @@
     <t>HDL_syntax/02_Jedi/security_flow/tst_06_encrypt_sub_module_lse</t>
   </si>
   <si>
-    <t>radiant=ng2_3</t>
-  </si>
-  <si>
-    <t>debug_10_reveal_inserter_v2.01</t>
-  </si>
-  <si>
     <t>HDL_syntax/00_device_flow/01_Thunderplus</t>
   </si>
   <si>
@@ -1391,6 +1385,21 @@
   </si>
   <si>
     <t>85</t>
+  </si>
+  <si>
+    <t>EIT2_case</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>EIT2_case/vm_rvl_syn</t>
+  </si>
+  <si>
+    <t>debug_10_reveal_inserter_v2.03</t>
+  </si>
+  <si>
+    <t>radiant=ng3_0</t>
   </si>
 </sst>
 </file>
@@ -5295,7 +5304,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A4822E2F-5A05-4643-84A4-810DB5F4877E}" diskRevisions="1" revisionId="530" version="12">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BF0B5910-C65C-4A8A-B34F-A9C9A736C8DA}" diskRevisions="1" revisionId="716" version="25">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5392,6 +5401,110 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{B538ED5E-46F1-48BC-896F-B09868CB21BA}" dateTime="2021-04-07T16:13:04" maxSheetId="5" userName="Jason Wang" r:id="rId13" minRId="531">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{34C44565-7DBA-4F33-B233-96B68C1325C2}" dateTime="2021-04-07T16:33:14" maxSheetId="5" userName="Jason Wang" r:id="rId14" minRId="532">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{66591183-A2C7-4A89-861D-248EF57B70C2}" dateTime="2021-04-07T16:33:30" maxSheetId="5" userName="Jason Wang" r:id="rId15" minRId="534">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{44551B4E-3D1E-46BD-903B-EE9749939EAF}" dateTime="2021-04-07T16:33:58" maxSheetId="5" userName="Jason Wang" r:id="rId16" minRId="536">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6057E85C-6986-459B-B35C-C9F3B1862B98}" dateTime="2021-04-07T16:34:17" maxSheetId="5" userName="Jason Wang" r:id="rId17" minRId="538" maxRId="539">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8F6BB5B2-6B11-41F1-81F3-BCFCCBA1DCDF}" dateTime="2021-04-07T16:34:21" maxSheetId="5" userName="Jason Wang" r:id="rId18">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{22229C87-AAAA-4955-A1DE-3ED51AC8D528}" dateTime="2021-04-07T16:34:29" maxSheetId="5" userName="Jason Wang" r:id="rId19" minRId="542">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{83F273B6-BB07-44F9-96D5-4E70F250D8C2}" dateTime="2021-04-07T16:35:10" maxSheetId="5" userName="Jason Wang" r:id="rId20" minRId="543">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6AA10395-D191-4936-BE28-F7DBBCFE449A}" dateTime="2021-04-07T16:48:59" maxSheetId="5" userName="Jason Wang" r:id="rId21" minRId="544" maxRId="545">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8F7AE725-3DF2-46C9-B6E1-03D43D623910}" dateTime="2021-04-07T16:49:05" maxSheetId="5" userName="Jason Wang" r:id="rId22">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E1379FDB-647E-4A9F-A83B-F37D3CF69A01}" dateTime="2021-04-07T16:49:29" maxSheetId="5" userName="Jason Wang" r:id="rId23" minRId="548" maxRId="630">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A5C5644B-FB38-4A38-9224-192114AD8D8C}" dateTime="2021-04-07T16:49:30" maxSheetId="5" userName="Jason Wang" r:id="rId24">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BF0B5910-C65C-4A8A-B34F-A9C9A736C8DA}" dateTime="2021-04-07T16:51:45" maxSheetId="5" userName="Jason Wang" r:id="rId25" minRId="633" maxRId="715">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -5632,6 +5745,130 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="531" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.01</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.02</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="532" sId="2">
+    <nc r="D88" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="534" sId="2">
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="536" sId="2">
+    <nc r="E88" t="inlineStr">
+      <is>
+        <t>EIT2_case/vm_rvl_syn</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="538" sId="2">
+    <nc r="S88" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="539" sId="2">
+    <nc r="O88" t="inlineStr">
+      <is>
+        <t>cmd= --run-par</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="542" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.02</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.03</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="2">
@@ -6174,6 +6411,1340 @@
     <formula>case!$A$2:$AD$2</formula>
   </rdn>
   <rcv guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="543" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng3_0</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="544" sId="2" numFmtId="30">
+    <nc r="F88">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="545" sId="2">
+    <oc r="O88" t="inlineStr">
+      <is>
+        <t>cmd= --run-par</t>
+      </is>
+    </oc>
+    <nc r="O88" t="inlineStr">
+      <is>
+        <t>cmd= --run-export-bitstream</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="548" sId="2">
+    <nc r="B87" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="549" sId="2">
+    <nc r="B86" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="550" sId="2">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="551" sId="2">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="552" sId="2">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="553" sId="2">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="554" sId="2">
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="555" sId="2">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="556" sId="2">
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="557" sId="2">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="558" sId="2">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="559" sId="2">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="560" sId="2">
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="561" sId="2">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="562" sId="2">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="563" sId="2">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="564" sId="2">
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="565" sId="2">
+    <nc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="566" sId="2">
+    <nc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="567" sId="2">
+    <nc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="568" sId="2">
+    <nc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="569" sId="2">
+    <nc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="570" sId="2">
+    <nc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="571" sId="2">
+    <nc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="572" sId="2">
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="573" sId="2">
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="574" sId="2">
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="575" sId="2">
+    <nc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="576" sId="2">
+    <nc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="577" sId="2">
+    <nc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="578" sId="2">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="579" sId="2">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="580" sId="2">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="581" sId="2">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="582" sId="2">
+    <nc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="583" sId="2">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="584" sId="2">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="585" sId="2">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="586" sId="2">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="587" sId="2">
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="588" sId="2">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="589" sId="2">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="590" sId="2">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="591" sId="2">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="592" sId="2">
+    <nc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="593" sId="2">
+    <nc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="594" sId="2">
+    <nc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="595" sId="2">
+    <nc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="596" sId="2">
+    <nc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="597" sId="2">
+    <nc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="598" sId="2">
+    <nc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="599" sId="2">
+    <nc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="600" sId="2">
+    <nc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="601" sId="2">
+    <nc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="602" sId="2">
+    <nc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="603" sId="2">
+    <nc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="604" sId="2">
+    <nc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="605" sId="2">
+    <nc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="606" sId="2">
+    <nc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="607" sId="2">
+    <nc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="608" sId="2">
+    <nc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="609" sId="2">
+    <nc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="610" sId="2">
+    <nc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="611" sId="2">
+    <nc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="612" sId="2">
+    <nc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="613" sId="2">
+    <nc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="614" sId="2">
+    <nc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="615" sId="2">
+    <nc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="616" sId="2">
+    <nc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="617" sId="2">
+    <nc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="618" sId="2">
+    <nc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="619" sId="2">
+    <nc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="620" sId="2">
+    <nc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="621" sId="2">
+    <nc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="622" sId="2">
+    <nc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="623" sId="2">
+    <nc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="624" sId="2">
+    <nc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="625" sId="2">
+    <nc r="B80" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="626" sId="2">
+    <nc r="B81" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="627" sId="2">
+    <nc r="B82" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="628" sId="2">
+    <nc r="B83" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="629" sId="2">
+    <nc r="B84" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="630" sId="2">
+    <nc r="B85" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="633" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rcc rId="634" sId="2">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+  <rcc rId="635" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B7"/>
+  </rcc>
+  <rcc rId="636" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B8"/>
+  </rcc>
+  <rcc rId="637" sId="2">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B9"/>
+  </rcc>
+  <rcc rId="638" sId="2">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B10"/>
+  </rcc>
+  <rcc rId="639" sId="2">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B11"/>
+  </rcc>
+  <rcc rId="640" sId="2">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B12"/>
+  </rcc>
+  <rcc rId="641" sId="2">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B13"/>
+  </rcc>
+  <rcc rId="642" sId="2">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B14"/>
+  </rcc>
+  <rcc rId="643" sId="2">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B15"/>
+  </rcc>
+  <rcc rId="644" sId="2">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B16"/>
+  </rcc>
+  <rcc rId="645" sId="2">
+    <oc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B17"/>
+  </rcc>
+  <rcc rId="646" sId="2">
+    <oc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B18"/>
+  </rcc>
+  <rcc rId="647" sId="2">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B19"/>
+  </rcc>
+  <rcc rId="648" sId="2">
+    <oc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B20"/>
+  </rcc>
+  <rcc rId="649" sId="2">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B21"/>
+  </rcc>
+  <rcc rId="650" sId="2">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B22"/>
+  </rcc>
+  <rcc rId="651" sId="2">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B23"/>
+  </rcc>
+  <rcc rId="652" sId="2">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B24"/>
+  </rcc>
+  <rcc rId="653" sId="2">
+    <oc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B25"/>
+  </rcc>
+  <rcc rId="654" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B26"/>
+  </rcc>
+  <rcc rId="655" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B27"/>
+  </rcc>
+  <rcc rId="656" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B28"/>
+  </rcc>
+  <rcc rId="657" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B29"/>
+  </rcc>
+  <rcc rId="658" sId="2">
+    <oc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B30"/>
+  </rcc>
+  <rcc rId="659" sId="2">
+    <oc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B31"/>
+  </rcc>
+  <rcc rId="660" sId="2">
+    <oc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B32"/>
+  </rcc>
+  <rcc rId="661" sId="2">
+    <oc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B33"/>
+  </rcc>
+  <rcc rId="662" sId="2">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="663" sId="2">
+    <oc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B35"/>
+  </rcc>
+  <rcc rId="664" sId="2">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="665" sId="2">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="666" sId="2">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="667" sId="2">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="668" sId="2">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+  <rcc rId="669" sId="2">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B41"/>
+  </rcc>
+  <rcc rId="670" sId="2">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B42"/>
+  </rcc>
+  <rcc rId="671" sId="2">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B43"/>
+  </rcc>
+  <rcc rId="672" sId="2">
+    <oc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B44"/>
+  </rcc>
+  <rcc rId="673" sId="2">
+    <oc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B45"/>
+  </rcc>
+  <rcc rId="674" sId="2">
+    <oc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B46"/>
+  </rcc>
+  <rcc rId="675" sId="2">
+    <oc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B47"/>
+  </rcc>
+  <rcc rId="676" sId="2">
+    <oc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B48"/>
+  </rcc>
+  <rcc rId="677" sId="2">
+    <oc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B49"/>
+  </rcc>
+  <rcc rId="678" sId="2">
+    <oc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B50"/>
+  </rcc>
+  <rcc rId="679" sId="2">
+    <oc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B51"/>
+  </rcc>
+  <rcc rId="680" sId="2">
+    <oc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B52"/>
+  </rcc>
+  <rcc rId="681" sId="2">
+    <oc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B53"/>
+  </rcc>
+  <rcc rId="682" sId="2">
+    <oc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B54"/>
+  </rcc>
+  <rcc rId="683" sId="2">
+    <oc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B55"/>
+  </rcc>
+  <rcc rId="684" sId="2">
+    <oc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B56"/>
+  </rcc>
+  <rcc rId="685" sId="2">
+    <oc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B57"/>
+  </rcc>
+  <rcc rId="686" sId="2">
+    <oc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B58"/>
+  </rcc>
+  <rcc rId="687" sId="2">
+    <oc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B59"/>
+  </rcc>
+  <rcc rId="688" sId="2">
+    <oc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B60"/>
+  </rcc>
+  <rcc rId="689" sId="2">
+    <oc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B61"/>
+  </rcc>
+  <rcc rId="690" sId="2">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B62"/>
+  </rcc>
+  <rcc rId="691" sId="2">
+    <oc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B63"/>
+  </rcc>
+  <rcc rId="692" sId="2">
+    <oc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B64"/>
+  </rcc>
+  <rcc rId="693" sId="2">
+    <oc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B65"/>
+  </rcc>
+  <rcc rId="694" sId="2">
+    <oc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B66"/>
+  </rcc>
+  <rcc rId="695" sId="2">
+    <oc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B67"/>
+  </rcc>
+  <rcc rId="696" sId="2">
+    <oc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B68"/>
+  </rcc>
+  <rcc rId="697" sId="2">
+    <oc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B69"/>
+  </rcc>
+  <rcc rId="698" sId="2">
+    <oc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B70"/>
+  </rcc>
+  <rcc rId="699" sId="2">
+    <oc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B71"/>
+  </rcc>
+  <rcc rId="700" sId="2">
+    <oc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B72"/>
+  </rcc>
+  <rcc rId="701" sId="2">
+    <oc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B73"/>
+  </rcc>
+  <rcc rId="702" sId="2">
+    <oc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B74"/>
+  </rcc>
+  <rcc rId="703" sId="2">
+    <oc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B75"/>
+  </rcc>
+  <rcc rId="704" sId="2">
+    <oc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B76"/>
+  </rcc>
+  <rcc rId="705" sId="2">
+    <oc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B77"/>
+  </rcc>
+  <rcc rId="706" sId="2">
+    <oc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B78"/>
+  </rcc>
+  <rcc rId="707" sId="2">
+    <oc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B79"/>
+  </rcc>
+  <rcc rId="708" sId="2">
+    <oc r="B80" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B80"/>
+  </rcc>
+  <rcc rId="709" sId="2">
+    <oc r="B81" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B81"/>
+  </rcc>
+  <rcc rId="710" sId="2">
+    <oc r="B82" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B82"/>
+  </rcc>
+  <rcc rId="711" sId="2">
+    <oc r="B83" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B83"/>
+  </rcc>
+  <rcc rId="712" sId="2">
+    <oc r="B84" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B84"/>
+  </rcc>
+  <rcc rId="713" sId="2">
+    <oc r="B85" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B85"/>
+  </rcc>
+  <rcc rId="714" sId="2">
+    <oc r="B86" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B86"/>
+  </rcc>
+  <rcc rId="715" sId="2">
+    <oc r="B87" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B87"/>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
 </revisions>
 </file>
 
@@ -9387,7 +10958,7 @@
         <v>256</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>426</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -9421,7 +10992,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>425</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -9442,23 +11013,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B3" sqref="B3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
     <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}">
       <selection activeCell="F20" sqref="F20"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -9471,14 +11042,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD87"/>
+  <dimension ref="A1:AD88"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11017,22 +12588,22 @@
     </row>
     <row r="84" spans="1:19">
       <c r="A84" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F84" s="2">
         <v>2</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="S84" s="2" t="s">
         <v>264</v>
@@ -11040,22 +12611,22 @@
     </row>
     <row r="85" spans="1:19">
       <c r="A85" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="F85" s="2">
         <v>2</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="S85" s="2" t="s">
         <v>264</v>
@@ -11063,22 +12634,22 @@
     </row>
     <row r="86" spans="1:19">
       <c r="A86" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F86" s="2">
         <v>2</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="S86" s="2" t="s">
         <v>264</v>
@@ -11086,24 +12657,44 @@
     </row>
     <row r="87" spans="1:19">
       <c r="A87" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F87" s="2">
         <v>2</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="S87" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
+      <c r="A88" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F88" s="2">
+        <v>2</v>
+      </c>
+      <c r="O88" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="S88" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -11111,30 +12702,30 @@
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A2:AD2"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="M60" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A83" sqref="A83:XFD83"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
       <autoFilter ref="A2:AD2"/>
@@ -13691,12 +15282,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
@@ -13776,6 +15367,9 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13787,9 +15381,6 @@
     <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
i412--scan dir issue fix
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/debug_10_reveal_inserter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\reveal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-12" yWindow="6300" windowWidth="28836" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
-  <calcPr calcId="122211" calcOnSave="0"/>
+  <calcPr calcId="122211"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" xWindow="725" yWindow="226" windowWidth="1821" windowHeight="1123" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="454">
   <si>
     <t>CaseInfo</t>
   </si>
@@ -1396,10 +1396,40 @@
     <t>EIT2_case/vm_rvl_syn</t>
   </si>
   <si>
-    <t>debug_10_reveal_inserter_v2.03</t>
-  </si>
-  <si>
     <t>radiant=ng3_0</t>
+  </si>
+  <si>
+    <t>EIT2_case/DNG-11576</t>
+  </si>
+  <si>
+    <t>EIT2_case/DNG-12196</t>
+  </si>
+  <si>
+    <t>EIT2_case/DNG-12432</t>
+  </si>
+  <si>
+    <t>EIT2_case/DNG-13341</t>
+  </si>
+  <si>
+    <t>EIT2_case/SOF-131242</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>debug_10_reveal_inserter_v2.04</t>
   </si>
 </sst>
 </file>
@@ -5304,7 +5334,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BF0B5910-C65C-4A8A-B34F-A9C9A736C8DA}" diskRevisions="1" revisionId="716" version="25">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E6F4DAAD-EBF1-426B-849D-120947BFE84D}" diskRevisions="1" revisionId="744" version="27">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5505,6 +5535,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{A86E4534-B233-429E-893B-41E729726A17}" dateTime="2022-06-02T14:25:12" maxSheetId="5" userName="Jason Wang" r:id="rId26" minRId="717" maxRId="741">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E6F4DAAD-EBF1-426B-849D-120947BFE84D}" dateTime="2022-06-02T14:26:51" maxSheetId="5" userName="Jason Wang" r:id="rId27" minRId="743">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -7738,6 +7784,205 @@
       </is>
     </oc>
     <nc r="B87"/>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="717" sId="2">
+    <nc r="E89" t="inlineStr">
+      <is>
+        <t>EIT2_case/DNG-11576</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="718" sId="2">
+    <nc r="E90" t="inlineStr">
+      <is>
+        <t>EIT2_case/DNG-12196</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="719" sId="2">
+    <nc r="E91" t="inlineStr">
+      <is>
+        <t>EIT2_case/DNG-12432</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="720" sId="2">
+    <nc r="E92" t="inlineStr">
+      <is>
+        <t>EIT2_case/DNG-13341</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="721" sId="2">
+    <nc r="E93" t="inlineStr">
+      <is>
+        <t>EIT2_case/SOF-131242</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="722" sId="2">
+    <nc r="D89" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="723" sId="2">
+    <nc r="D90" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="724" sId="2">
+    <nc r="D91" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="725" sId="2">
+    <nc r="D92" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="726" sId="2">
+    <nc r="D93" t="inlineStr">
+      <is>
+        <t>EIT2_case</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="727" sId="2">
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>87</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="728" sId="2">
+    <nc r="A90" t="inlineStr">
+      <is>
+        <t>88</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="729" sId="2">
+    <nc r="A91" t="inlineStr">
+      <is>
+        <t>89</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="730" sId="2">
+    <nc r="A92" t="inlineStr">
+      <is>
+        <t>90</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="731" sId="2">
+    <nc r="A93" t="inlineStr">
+      <is>
+        <t>91</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="732" sId="2" numFmtId="30">
+    <nc r="F89">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="733" sId="2" numFmtId="30">
+    <nc r="F90">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="734" sId="2" numFmtId="30">
+    <nc r="F91">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="735" sId="2" numFmtId="30">
+    <nc r="F92">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="736" sId="2" numFmtId="30">
+    <nc r="F93">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="737" sId="2">
+    <nc r="S89" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="738" sId="2">
+    <nc r="S90" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="739" sId="2">
+    <nc r="S91" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="740" sId="2">
+    <nc r="S92" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="741" sId="2">
+    <nc r="S93" t="inlineStr">
+      <is>
+        <t>reveal</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="743" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.03</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>debug_10_reveal_inserter_v2.04</t>
+      </is>
+    </nc>
   </rcc>
   <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
@@ -10928,9 +11173,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
@@ -10958,7 +11205,7 @@
         <v>256</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -10992,7 +11239,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -11014,7 +11261,7 @@
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -11042,46 +11289,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD88"/>
+  <dimension ref="A1:AD93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
     <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="11" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" customWidth="1"/>
     <col min="23" max="28" width="9" style="2"/>
-    <col min="29" max="29" width="10.140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="10.109375" style="2" customWidth="1"/>
     <col min="30" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A1" s="67" t="s">
         <v>12</v>
       </c>
@@ -11117,7 +11364,7 @@
       <c r="AC1" s="70"/>
       <c r="AD1" s="70"/>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -11209,7 +11456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" thickTop="1">
+    <row r="3" spans="1:30" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>261</v>
       </c>
@@ -12695,6 +12942,91 @@
         <v>434</v>
       </c>
       <c r="S88" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
+      <c r="A89" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F89" s="2">
+        <v>2</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
+      <c r="A90" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="F90" s="2">
+        <v>2</v>
+      </c>
+      <c r="S90" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="A91" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="F91" s="2">
+        <v>2</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="A92" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F92" s="2">
+        <v>2</v>
+      </c>
+      <c r="S92" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
+      <c r="A93" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="F93" s="2">
+        <v>2</v>
+      </c>
+      <c r="S93" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -12703,8 +13035,8 @@
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A2:AD2"/>
@@ -12811,18 +13143,18 @@
       <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -12845,7 +13177,7 @@
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="108" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="109" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="110" spans="1:14" ht="15.75" thickBot="1">
+    <row r="110" spans="1:14" ht="15" thickBot="1">
       <c r="A110" s="6" t="s">
         <v>71</v>
       </c>
@@ -12853,7 +13185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" thickBot="1">
+    <row r="111" spans="1:14" ht="15" thickBot="1">
       <c r="A111" s="9" t="s">
         <v>73</v>
       </c>
@@ -13681,7 +14013,7 @@
       <c r="M141" s="18"/>
       <c r="N141" s="19"/>
     </row>
-    <row r="142" spans="1:14" ht="15.75" thickBot="1">
+    <row r="142" spans="1:14" ht="15" thickBot="1">
       <c r="A142" s="20" t="s">
         <v>112</v>
       </c>
@@ -13705,7 +14037,7 @@
       <c r="M142" s="21"/>
       <c r="N142" s="22"/>
     </row>
-    <row r="145" spans="1:8" ht="15.75" thickBot="1">
+    <row r="145" spans="1:8" ht="15" thickBot="1">
       <c r="A145" s="6" t="s">
         <v>113</v>
       </c>
@@ -14323,7 +14655,7 @@
       </c>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" ht="90">
+    <row r="173" spans="1:8" ht="86.4">
       <c r="A173" s="26">
         <v>27</v>
       </c>
@@ -14417,7 +14749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="15.75" thickBot="1">
+    <row r="177" spans="1:8" ht="15" thickBot="1">
       <c r="A177" s="31">
         <v>31</v>
       </c>
@@ -14573,7 +14905,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="15.75" thickBot="1">
+    <row r="184" spans="1:8" ht="15" thickBot="1">
       <c r="A184" s="35">
         <v>38</v>
       </c>
@@ -14613,7 +14945,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15.75" thickBot="1">
+    <row r="197" spans="1:7" ht="15" thickBot="1">
       <c r="A197" s="6" t="s">
         <v>197</v>
       </c>
@@ -14887,7 +15219,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15.75" thickBot="1">
+    <row r="214" spans="1:7" ht="15" thickBot="1">
       <c r="A214" s="96"/>
       <c r="B214" s="97"/>
       <c r="C214" s="97" t="s">
@@ -14921,7 +15253,7 @@
       <c r="D217" s="37"/>
       <c r="E217" s="37"/>
     </row>
-    <row r="218" spans="1:7" ht="15.75" thickBot="1">
+    <row r="218" spans="1:7" ht="15" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>221</v>
       </c>
@@ -14929,7 +15261,7 @@
       <c r="D218" s="37"/>
       <c r="E218" s="37"/>
     </row>
-    <row r="219" spans="1:7" ht="15.75" thickBot="1">
+    <row r="219" spans="1:7" ht="15" thickBot="1">
       <c r="A219" s="45" t="s">
         <v>222</v>
       </c>
@@ -15017,12 +15349,12 @@
     <row r="224" spans="1:7">
       <c r="C224" s="51"/>
     </row>
-    <row r="226" spans="1:7" ht="15.75" thickBot="1">
+    <row r="226" spans="1:7" ht="15" thickBot="1">
       <c r="A226" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15.75" thickBot="1">
+    <row r="227" spans="1:7" ht="15" thickBot="1">
       <c r="A227" s="9" t="s">
         <v>233</v>
       </c>
@@ -15262,7 +15594,7 @@
       <c r="F240" s="64"/>
       <c r="G240" s="43"/>
     </row>
-    <row r="241" spans="1:7" ht="15.75" thickBot="1">
+    <row r="241" spans="1:7" ht="15" thickBot="1">
       <c r="A241" s="65">
         <v>44118</v>
       </c>
@@ -15358,7 +15690,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>